<commit_message>
make exe with a more generic approach
</commit_message>
<xml_diff>
--- a/Bierlisten/Bierliste_K31_12.01.2020.xlsx
+++ b/Bierlisten/Bierliste_K31_12.01.2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\Projekte\Python\Bierliste_K3.1\Bierlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB13EBE-D045-4B2A-A72D-61169A6305A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2435200F-A3A2-432A-888A-54FA62CEC088}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>Getränkeliste Küche 3.1</t>
   </si>
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,12 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -416,7 +410,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -429,7 +422,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -441,6 +433,32 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,12 +762,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2200,12 +2218,12 @@
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="10" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" style="1" customWidth="1"/>
@@ -2219,12 +2237,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2268,564 +2286,565 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="26">
+        <v>311</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="20">
         <v>11.3</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22">
         <v>404</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22">
         <v>106</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="27">
+        <v>312</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="16">
         <v>-1.6000000000000161</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18">
         <v>467</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18">
         <v>86</v>
       </c>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="28">
+        <v>313</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="12">
+        <v>-10.050000000000001</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14">
+        <v>58</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14">
+        <v>9</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>314</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="16">
+        <v>-1.05</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18">
+        <v>45</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18">
+        <v>2</v>
+      </c>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>315</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="12">
+        <v>-3.9499999999999988</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14">
+        <v>238</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14">
+        <v>170</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>316</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="16">
+        <v>62.5</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18">
+        <v>227</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18">
+        <v>103</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>317</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14">
+        <v>58</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14">
+        <v>19</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>318</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16">
+        <v>-30.65</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18">
+        <v>577</v>
+      </c>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18">
+        <v>261</v>
+      </c>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
+        <v>319</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="12">
+        <v>3.9</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14">
+        <v>65</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14">
+        <v>11</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>349</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="16">
+        <v>-37.85</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18">
+        <v>182</v>
+      </c>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18">
+        <v>57</v>
+      </c>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>310</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="12">
+        <v>-16.8</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14">
+        <v>154</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14">
+        <v>47</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="16">
+        <v>-2.2500000000000009</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18">
+        <v>369</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18">
+        <v>28</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="12">
+        <v>-17.100000000000001</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14">
+        <v>83</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18">
+        <v>3</v>
+      </c>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="12">
+        <v>-0.9</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>340</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="16">
+        <v>-9</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18">
+        <v>2</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
         <v>20</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B19" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="12">
+        <v>-1.8</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>230</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="16">
+        <v>-2.7</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+    </row>
+    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
+        <v>225</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12">
+        <v>-0.9</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <v>123</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="16">
+        <v>-0.9</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+    </row>
+    <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28">
+        <v>118</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="12">
+        <v>-0.9</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>230</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="16">
+        <v>-1.8</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+    </row>
+    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28">
+        <v>316</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14">
         <v>21</v>
       </c>
-      <c r="C5" s="16">
-        <v>-10.050000000000001</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18">
-        <v>58</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18">
-        <v>9</v>
-      </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="21">
-        <v>-1.05</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23">
-        <v>45</v>
-      </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23">
+      <c r="J25" s="14"/>
+      <c r="K25" s="14">
         <v>2</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="16">
-        <v>-3.9499999999999988</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18">
-        <v>238</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18">
-        <v>170</v>
-      </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="21">
-        <v>62.5</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23">
-        <v>227</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23">
-        <v>103</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="16">
-        <v>2.7</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18">
-        <v>58</v>
-      </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18">
-        <v>19</v>
-      </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="21">
-        <v>-30.65</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23">
-        <v>577</v>
-      </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23">
-        <v>261</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="16">
-        <v>3.9</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18">
-        <v>65</v>
-      </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18">
-        <v>11</v>
-      </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="21">
-        <v>-37.85</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23">
-        <v>182</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23">
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
+        <v>215</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="16">
-        <v>-16.8</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18">
-        <v>154</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18">
-        <v>47</v>
-      </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="21">
-        <v>-2.2500000000000009</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23">
-        <v>369</v>
-      </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23">
-        <v>28</v>
-      </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-    </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="16">
-        <v>-17.100000000000001</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18">
-        <v>83</v>
-      </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23">
-        <v>3</v>
-      </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-    </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="C26" s="16">
         <v>-0.9</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="21">
-        <v>-9</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23">
-        <v>2</v>
-      </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="16">
-        <v>-1.8</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-    </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="21">
-        <v>-2.7</v>
-      </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-    </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="16">
-        <v>-0.9</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="21">
-        <v>-0.9</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-    </row>
-    <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="16">
-        <v>-0.9</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-    </row>
-    <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="21">
-        <v>-1.8</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-    </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="18">
-        <v>21</v>
-      </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18">
-        <v>2</v>
-      </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-    </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
-        <v>215</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="21">
-        <v>-0.9</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
       <c r="B27" s="10"/>
       <c r="C27" s="7"/>
       <c r="I27" s="8"/>
@@ -2835,6 +2854,7 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
       <c r="B28" s="10"/>
       <c r="C28" s="7"/>
       <c r="I28" s="8"/>
@@ -2844,6 +2864,7 @@
       <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
       <c r="B29" s="10"/>
       <c r="C29" s="7"/>
       <c r="I29" s="8"/>
@@ -2853,6 +2874,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
       <c r="B30" s="10"/>
       <c r="C30" s="7"/>
       <c r="I30" s="8"/>
@@ -2862,6 +2884,7 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
       <c r="B31" s="10"/>
       <c r="C31" s="7"/>
       <c r="I31" s="8"/>
@@ -2871,6 +2894,7 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
       <c r="B32" s="10"/>
       <c r="C32" s="7"/>
       <c r="I32" s="8"/>
@@ -2879,7 +2903,8 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
     </row>
-    <row r="33" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
       <c r="B33" s="10"/>
       <c r="C33" s="7"/>
       <c r="I33" s="8"/>
@@ -2888,7 +2913,8 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
     </row>
-    <row r="34" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
       <c r="B34" s="10"/>
       <c r="C34" s="7"/>
       <c r="I34" s="8"/>
@@ -2897,7 +2923,8 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
     </row>
-    <row r="35" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
       <c r="B35" s="10"/>
       <c r="C35" s="7"/>
       <c r="I35" s="8"/>
@@ -2906,7 +2933,8 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
       <c r="B36" s="10"/>
       <c r="C36" s="7"/>
       <c r="I36" s="8"/>
@@ -2915,7 +2943,8 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
     </row>
-    <row r="37" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="29"/>
       <c r="B37" s="10"/>
       <c r="C37" s="7"/>
       <c r="I37" s="8"/>
@@ -2924,7 +2953,8 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
     </row>
-    <row r="38" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="29"/>
       <c r="B38" s="10"/>
       <c r="C38" s="7"/>
       <c r="I38" s="8"/>
@@ -2933,7 +2963,8 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
     </row>
-    <row r="39" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
       <c r="B39" s="10"/>
       <c r="C39" s="7"/>
       <c r="I39" s="8"/>
@@ -2942,7 +2973,8 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
     </row>
-    <row r="40" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
       <c r="B40" s="10"/>
       <c r="C40" s="7"/>
       <c r="I40" s="8"/>
@@ -2951,7 +2983,8 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
     </row>
-    <row r="41" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
       <c r="B41" s="10"/>
       <c r="C41" s="7"/>
       <c r="I41" s="8"/>
@@ -2960,7 +2993,8 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="29"/>
       <c r="B42" s="10"/>
       <c r="C42" s="7"/>
       <c r="I42" s="8"/>
@@ -2969,7 +3003,8 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
       <c r="B43" s="10"/>
       <c r="C43" s="7"/>
       <c r="I43" s="8"/>
@@ -2978,7 +3013,8 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
     </row>
-    <row r="44" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
       <c r="B44" s="10"/>
       <c r="C44" s="7"/>
       <c r="I44" s="8"/>
@@ -2987,7 +3023,8 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
     </row>
-    <row r="45" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="29"/>
       <c r="B45" s="10"/>
       <c r="C45" s="7"/>
       <c r="I45" s="8"/>
@@ -2996,7 +3033,8 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="46" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="29"/>
       <c r="B46" s="10"/>
       <c r="C46" s="7"/>
       <c r="I46" s="8"/>
@@ -3005,7 +3043,8 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
     </row>
-    <row r="47" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="29"/>
       <c r="B47" s="10"/>
       <c r="C47" s="7"/>
       <c r="I47" s="8"/>
@@ -3014,7 +3053,8 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
     </row>
-    <row r="48" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="29"/>
       <c r="B48" s="10"/>
       <c r="C48" s="7"/>
       <c r="I48" s="8"/>
@@ -3023,7 +3063,8 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="29"/>
       <c r="B49" s="10"/>
       <c r="C49" s="7"/>
       <c r="I49" s="8"/>
@@ -3032,7 +3073,8 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
     </row>
-    <row r="50" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="29"/>
       <c r="B50" s="10"/>
       <c r="C50" s="7"/>
       <c r="I50" s="8"/>
@@ -3041,7 +3083,8 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="29"/>
       <c r="B51" s="10"/>
       <c r="C51" s="7"/>
       <c r="I51" s="8"/>
@@ -3050,7 +3093,8 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
-    <row r="52" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="29"/>
       <c r="B52" s="10"/>
       <c r="C52" s="7"/>
       <c r="I52" s="8"/>
@@ -3059,7 +3103,8 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
     </row>
-    <row r="53" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="29"/>
       <c r="B53" s="10"/>
       <c r="C53" s="7"/>
       <c r="I53" s="8"/>
@@ -3068,7 +3113,8 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
     </row>
-    <row r="54" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="29"/>
       <c r="B54" s="10"/>
       <c r="C54" s="7"/>
       <c r="I54" s="8"/>
@@ -3077,7 +3123,8 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="29"/>
       <c r="B55" s="10"/>
       <c r="C55" s="7"/>
       <c r="I55" s="8"/>
@@ -3086,7 +3133,8 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="29"/>
       <c r="B56" s="10"/>
       <c r="C56" s="7"/>
       <c r="I56" s="8"/>
@@ -3095,7 +3143,8 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
     </row>
-    <row r="57" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="29"/>
       <c r="B57" s="10"/>
       <c r="C57" s="7"/>
       <c r="I57" s="8"/>
@@ -3104,7 +3153,8 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
     </row>
-    <row r="58" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="29"/>
       <c r="B58" s="10"/>
       <c r="C58" s="7"/>
       <c r="I58" s="8"/>
@@ -3113,7 +3163,8 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
-    <row r="59" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="29"/>
       <c r="B59" s="10"/>
       <c r="C59" s="7"/>
       <c r="I59" s="8"/>
@@ -3122,7 +3173,8 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
     </row>
-    <row r="60" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
       <c r="B60" s="10"/>
       <c r="C60" s="7"/>
       <c r="I60" s="8"/>
@@ -3131,7 +3183,8 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
       <c r="B61" s="10"/>
       <c r="C61" s="7"/>
       <c r="I61" s="8"/>
@@ -3140,7 +3193,8 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="29"/>
       <c r="B62" s="10"/>
       <c r="C62" s="7"/>
       <c r="I62" s="8"/>
@@ -3149,7 +3203,8 @@
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="29"/>
       <c r="B63" s="10"/>
       <c r="C63" s="7"/>
       <c r="I63" s="8"/>
@@ -3158,7 +3213,8 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="29"/>
       <c r="B64" s="10"/>
       <c r="C64" s="7"/>
       <c r="I64" s="8"/>
@@ -3167,7 +3223,8 @@
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
     </row>
-    <row r="65" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="29"/>
       <c r="B65" s="10"/>
       <c r="C65" s="7"/>
       <c r="I65" s="8"/>
@@ -3176,7 +3233,8 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
     </row>
-    <row r="66" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="29"/>
       <c r="B66" s="10"/>
       <c r="C66" s="7"/>
       <c r="I66" s="8"/>
@@ -3185,7 +3243,8 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="29"/>
       <c r="B67" s="10"/>
       <c r="C67" s="7"/>
       <c r="I67" s="8"/>

</xml_diff>